<commit_message>
expanded neighborhood to include not feasible
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacopx/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20560"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -85,11 +80,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +108,14 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -375,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -418,15 +421,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -718,45 +725,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:X14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.33203125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" style="4" customWidth="1"/>
-    <col min="21" max="21" width="11.33203125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" style="4" customWidth="1"/>
-    <col min="23" max="23" width="11.33203125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="11.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.36328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.36328125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="11.36328125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.36328125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="11.36328125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.36328125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="11.36328125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11.36328125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="11.36328125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.36328125" style="4" customWidth="1"/>
+    <col min="21" max="21" width="11.36328125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="11.36328125" style="4" customWidth="1"/>
+    <col min="23" max="23" width="11.36328125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="11.36328125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" s="27" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I2" s="27">
+    <row r="2" spans="1:24" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I2" s="28">
         <v>43075</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6"/>
       <c r="B3" s="18" t="s">
         <v>0</v>
@@ -825,7 +832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
@@ -848,11 +855,11 @@
         <v>157.03273300000001</v>
       </c>
       <c r="I4" s="23">
-        <v>166.29599999999999</v>
+        <v>169.42500000000001</v>
       </c>
       <c r="J4" s="24">
         <f t="shared" ref="J4:J10" si="0">100*(I4-G4)/G4</f>
-        <v>5.8989401910237307</v>
+        <v>7.8915183880802759</v>
       </c>
       <c r="K4" s="23"/>
       <c r="L4" s="24" t="e">
@@ -890,7 +897,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
@@ -913,11 +920,11 @@
         <v>34.708820000000003</v>
       </c>
       <c r="I5" s="22">
-        <v>56.606999999999999</v>
+        <v>45.341000000000001</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" si="0"/>
-        <v>63.09111055921808</v>
+        <v>30.632502055673449</v>
       </c>
       <c r="K5" s="22"/>
       <c r="L5" s="24" t="e">
@@ -955,7 +962,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>6</v>
       </c>
@@ -978,11 +985,11 @@
         <v>32.626666999999998</v>
       </c>
       <c r="I6" s="22">
-        <v>62.398000000000003</v>
+        <v>49.561</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="0"/>
-        <v>91.248465557330775</v>
+        <v>51.903349490157858</v>
       </c>
       <c r="K6" s="22"/>
       <c r="L6" s="24" t="e">
@@ -1020,7 +1027,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
@@ -1043,11 +1050,11 @@
         <v>7.7172020000000003</v>
       </c>
       <c r="I7" s="22">
-        <v>14.194000000000001</v>
+        <v>11.500999999999999</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
-        <v>83.926765166960763</v>
+        <v>49.030697913570215</v>
       </c>
       <c r="K7" s="22"/>
       <c r="L7" s="24" t="e">
@@ -1085,7 +1092,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>8</v>
       </c>
@@ -1108,11 +1115,11 @@
         <v>12.901103000000001</v>
       </c>
       <c r="I8" s="22">
-        <v>28.725000000000001</v>
+        <v>18.212</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>122.65538070659538</v>
+        <v>41.166224314308614</v>
       </c>
       <c r="K8" s="22"/>
       <c r="L8" s="24" t="e">
@@ -1150,7 +1157,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
         <v>9</v>
       </c>
@@ -1172,10 +1179,12 @@
       <c r="G9" s="10">
         <v>3.044578</v>
       </c>
-      <c r="I9" s="22"/>
+      <c r="I9" s="22">
+        <v>4.6239999999999997</v>
+      </c>
       <c r="J9" s="3">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>51.87654906525632</v>
       </c>
       <c r="K9" s="22"/>
       <c r="L9" s="24" t="e">
@@ -1213,7 +1222,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="17" t="s">
         <v>10</v>
       </c>
@@ -1236,11 +1245,11 @@
         <v>10.050300999999999</v>
       </c>
       <c r="I10" s="22">
-        <v>19</v>
+        <v>12.855</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>89.049064301656244</v>
+        <v>27.906616926199536</v>
       </c>
       <c r="K10" s="22"/>
       <c r="L10" s="24" t="e">
@@ -1278,13 +1287,13 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="I12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J12" s="4">
         <f>MIN(J4:J10)</f>
-        <v>-100</v>
+        <v>7.8915183880802759</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>14</v>
@@ -1336,13 +1345,13 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="I13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J13" s="4">
         <f>AVERAGE(J4:J10)</f>
-        <v>50.838532354683572</v>
+        <v>37.201065450463751</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>15</v>
@@ -1394,13 +1403,13 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="I14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="J14" s="4">
         <f>MAX(J4:J10)</f>
-        <v>122.65538070659538</v>
+        <v>51.903349490157858</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>16</v>
@@ -1454,17 +1463,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1472,12 +1481,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
added also annailing 2
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -731,7 +731,7 @@
   <dimension ref="A2:X14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -864,11 +864,11 @@
         <v>6.3472543651137956</v>
       </c>
       <c r="K4" s="23">
-        <v>157</v>
+        <v>158.1</v>
       </c>
       <c r="L4" s="24">
         <f>100*(K4-$G$4)/K4</f>
-        <v>-2.0849044585992006E-2</v>
+        <v>0.67505819101833453</v>
       </c>
       <c r="M4" s="23"/>
       <c r="N4" s="24" t="e">
@@ -930,10 +930,12 @@
         <f t="shared" si="0"/>
         <v>30.632502055673449</v>
       </c>
-      <c r="K5" s="22"/>
-      <c r="L5" s="24" t="e">
-        <f>100*(K5-$G$4)/K5</f>
-        <v>#DIV/0!</v>
+      <c r="K5" s="22">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="L5" s="24">
+        <f>100*(K5-$G$5)/K5</f>
+        <v>14.929362745098027</v>
       </c>
       <c r="M5" s="22"/>
       <c r="N5" s="24" t="e">
@@ -995,10 +997,12 @@
         <f t="shared" si="0"/>
         <v>49.748670313152125</v>
       </c>
-      <c r="K6" s="22"/>
-      <c r="L6" s="24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="K6" s="22">
+        <v>38.659999999999997</v>
+      </c>
+      <c r="L6" s="24">
+        <f>100*(K6-$G$6)/K6</f>
+        <v>15.60613812726332</v>
       </c>
       <c r="M6" s="22"/>
       <c r="N6" s="24" t="e">
@@ -1060,10 +1064,12 @@
         <f t="shared" si="0"/>
         <v>49.030697913570215</v>
       </c>
-      <c r="K7" s="22"/>
-      <c r="L7" s="24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="K7" s="22">
+        <v>9.1519999999999992</v>
+      </c>
+      <c r="L7" s="24">
+        <f>100*(K7-$G$7)/K7</f>
+        <v>15.67742569930069</v>
       </c>
       <c r="M7" s="22"/>
       <c r="N7" s="24" t="e">
@@ -1125,10 +1131,12 @@
         <f t="shared" si="0"/>
         <v>40.59262994799748</v>
       </c>
-      <c r="K8" s="22"/>
-      <c r="L8" s="24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="K8" s="22">
+        <v>15.734</v>
+      </c>
+      <c r="L8" s="24">
+        <f>100*(K8-$G$8)/K8</f>
+        <v>18.004938350069907</v>
       </c>
       <c r="M8" s="22"/>
       <c r="N8" s="24" t="e">
@@ -1191,11 +1199,11 @@
         <v>51.87654906525632</v>
       </c>
       <c r="K9" s="22">
-        <v>3.7869999999999999</v>
+        <v>3.653</v>
       </c>
       <c r="L9" s="24">
         <f>100*(K9-$G$9)/K9</f>
-        <v>19.604489041457619</v>
+        <v>16.655406515192993</v>
       </c>
       <c r="M9" s="22"/>
       <c r="N9" s="24" t="e">
@@ -1257,10 +1265,12 @@
         <f t="shared" si="0"/>
         <v>39.866457730967475</v>
       </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="K10" s="22">
+        <v>12.5</v>
+      </c>
+      <c r="L10" s="24">
+        <f>100*(K10-$G$10)/K10</f>
+        <v>19.597592000000006</v>
       </c>
       <c r="M10" s="22"/>
       <c r="N10" s="24" t="e">
@@ -1304,9 +1314,9 @@
       <c r="K12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="4" t="e">
+      <c r="L12" s="4">
         <f t="shared" ref="L12" si="32">MIN(L4:L10)</f>
-        <v>#DIV/0!</v>
+        <v>0.67505819101833453</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>14</v>
@@ -1362,9 +1372,9 @@
       <c r="K13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="4" t="e">
+      <c r="L13" s="4">
         <f t="shared" ref="L13" si="39">AVERAGE(L4:L10)</f>
-        <v>#DIV/0!</v>
+        <v>14.449417375420468</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>15</v>
@@ -1420,9 +1430,9 @@
       <c r="K14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L14" s="4" t="e">
+      <c r="L14" s="4">
         <f t="shared" ref="L14" si="46">MAX(L4:L10)</f>
-        <v>#DIV/0!</v>
+        <v>19.597592000000006</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
local swap in loop
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -864,21 +864,25 @@
         <v>6.3472543651137956</v>
       </c>
       <c r="K4" s="23">
-        <v>158.072</v>
+        <v>157.654</v>
       </c>
       <c r="L4" s="24">
         <f>100*(K4-$G$4)/K4</f>
-        <v>0.65746432005667998</v>
-      </c>
-      <c r="M4" s="23"/>
-      <c r="N4" s="24" t="e">
-        <f>100*(M4-$G$4)/M4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O4" s="23"/>
-      <c r="P4" s="24" t="e">
+        <v>0.39406992527940232</v>
+      </c>
+      <c r="M4" s="23">
+        <v>157.14500000000001</v>
+      </c>
+      <c r="N4" s="24">
+        <f>100*(M4-G4)/M4</f>
+        <v>7.1441662159154137E-2</v>
+      </c>
+      <c r="O4" s="23">
+        <v>157.14500000000001</v>
+      </c>
+      <c r="P4" s="24">
         <f>100*(O4-$G$4)/O4</f>
-        <v>#DIV/0!</v>
+        <v>7.1441662159154137E-2</v>
       </c>
       <c r="Q4" s="23"/>
       <c r="R4" s="24" t="e">
@@ -937,15 +941,19 @@
         <f>100*(K5-$G$5)/K5</f>
         <v>13.093244529019978</v>
       </c>
-      <c r="M5" s="22"/>
-      <c r="N5" s="24" t="e">
-        <f t="shared" ref="L5:N10" si="1">100*(M5-$G$4)/M5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O5" s="22"/>
-      <c r="P5" s="24" t="e">
+      <c r="M5" s="22">
+        <v>38.816000000000003</v>
+      </c>
+      <c r="N5" s="24">
+        <f t="shared" ref="N5:N10" si="1">100*(M5-G5)/M5</f>
+        <v>10.581152102225884</v>
+      </c>
+      <c r="O5" s="22">
+        <v>38.816000000000003</v>
+      </c>
+      <c r="P5" s="24">
         <f t="shared" ref="P5" si="2">100*(O5-$G$4)/O5</f>
-        <v>#DIV/0!</v>
+        <v>-304.55671115004122</v>
       </c>
       <c r="Q5" s="22"/>
       <c r="R5" s="24" t="e">
@@ -998,11 +1006,11 @@
         <v>49.748670313152125</v>
       </c>
       <c r="K6" s="22">
-        <v>38.462000000000003</v>
+        <v>37.414999999999999</v>
       </c>
       <c r="L6" s="24">
         <f>100*(K6-$G$6)/K6</f>
-        <v>15.171683739795135</v>
+        <v>12.79789656554858</v>
       </c>
       <c r="M6" s="22"/>
       <c r="N6" s="24" t="e">
@@ -1065,11 +1073,11 @@
         <v>49.030697913570215</v>
       </c>
       <c r="K7" s="22">
-        <v>9.0890000000000004</v>
+        <v>8.9920000000000009</v>
       </c>
       <c r="L7" s="24">
         <f>100*(K7-$G$7)/K7</f>
-        <v>15.092947518978985</v>
+        <v>14.177024021352318</v>
       </c>
       <c r="M7" s="22"/>
       <c r="N7" s="24" t="e">
@@ -1132,11 +1140,11 @@
         <v>40.59262994799748</v>
       </c>
       <c r="K8" s="22">
-        <v>15.638</v>
+        <v>15.346</v>
       </c>
       <c r="L8" s="24">
         <f>100*(K8-$G$8)/K8</f>
-        <v>17.501579485867751</v>
+        <v>15.931819366610187</v>
       </c>
       <c r="M8" s="22"/>
       <c r="N8" s="24" t="e">
@@ -1199,11 +1207,11 @@
         <v>51.87654906525632</v>
       </c>
       <c r="K9" s="22">
-        <v>3.6389999999999998</v>
+        <v>3.645</v>
       </c>
       <c r="L9" s="24">
         <f>100*(K9-$G$9)/K9</f>
-        <v>16.334762297334429</v>
+        <v>16.472482853223593</v>
       </c>
       <c r="M9" s="22"/>
       <c r="N9" s="24" t="e">
@@ -1266,16 +1274,18 @@
         <v>39.866457730967475</v>
       </c>
       <c r="K10" s="22">
-        <v>11.926</v>
+        <v>11.225</v>
       </c>
       <c r="L10" s="24">
         <f>100*(K10-$G$10)/K10</f>
-        <v>15.727813181284594</v>
-      </c>
-      <c r="M10" s="22"/>
-      <c r="N10" s="24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>10.465024498886418</v>
+      </c>
+      <c r="M10" s="22">
+        <v>11.007999999999999</v>
+      </c>
+      <c r="N10" s="24">
+        <f>100*(M10-G10)/M10</f>
+        <v>8.7000272529069758</v>
       </c>
       <c r="O10" s="22"/>
       <c r="P10" s="24" t="e">
@@ -1316,7 +1326,7 @@
       </c>
       <c r="L12" s="4">
         <f t="shared" ref="L12" si="32">MIN(L4:L10)</f>
-        <v>0.65746432005667998</v>
+        <v>0.39406992527940232</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>14</v>
@@ -1374,7 +1384,7 @@
       </c>
       <c r="L13" s="4">
         <f t="shared" ref="L13" si="39">AVERAGE(L4:L10)</f>
-        <v>13.368499296048219</v>
+        <v>11.904508822845782</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>15</v>
@@ -1432,7 +1442,7 @@
       </c>
       <c r="L14" s="4">
         <f t="shared" ref="L14" si="46">MAX(L4:L10)</f>
-        <v>17.501579485867751</v>
+        <v>16.472482853223593</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Adding benchmark (from prof) and benchmark-history
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="29005"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacopx/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="440" windowWidth="18740" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Exams</t>
   </si>
@@ -75,16 +80,22 @@
   </si>
   <si>
     <t>Worst:</t>
+  </si>
+  <si>
+    <t>Your algorithm best solution obj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill the green cells only!!! Do not change anything else!!! </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,27 +114,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -386,56 +389,53 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -727,45 +727,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:X14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.36328125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="11.36328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.36328125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="11.36328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.36328125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="11.36328125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.36328125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="11.36328125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.36328125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="11.36328125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="11.36328125" style="4" customWidth="1"/>
-    <col min="21" max="21" width="11.36328125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="11.36328125" style="4" customWidth="1"/>
-    <col min="23" max="23" width="11.36328125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="11.36328125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="32.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I2" s="28">
-        <v>43075</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
+    </row>
+    <row r="2" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="18" t="s">
         <v>0</v>
@@ -785,56 +781,14 @@
       <c r="G3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="26">
-        <v>1</v>
-      </c>
-      <c r="J3" s="25" t="s">
+      <c r="I3" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="26">
-        <v>2</v>
-      </c>
-      <c r="L3" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3" s="26">
-        <v>3</v>
-      </c>
-      <c r="N3" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="26">
-        <v>4</v>
-      </c>
-      <c r="P3" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" s="26">
-        <v>5</v>
-      </c>
-      <c r="R3" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="S3" s="26">
-        <v>6</v>
-      </c>
-      <c r="T3" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="U3" s="26">
-        <v>7</v>
-      </c>
-      <c r="V3" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="W3" s="26">
-        <v>8</v>
-      </c>
-      <c r="X3" s="25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
@@ -857,55 +811,14 @@
         <v>157.03273300000001</v>
       </c>
       <c r="I4" s="23">
-        <v>167</v>
+        <v>157.08099999999999</v>
       </c>
       <c r="J4" s="24">
-        <f t="shared" ref="J4:J10" si="0">100*(I4-G4)/G4</f>
-        <v>6.3472543651137956</v>
-      </c>
-      <c r="K4" s="23">
-        <v>157.654</v>
-      </c>
-      <c r="L4" s="24">
-        <f>100*(K4-$G$4)/K4</f>
-        <v>0.39406992527940232</v>
-      </c>
-      <c r="M4" s="23">
-        <v>157.14500000000001</v>
-      </c>
-      <c r="N4" s="24">
-        <f>100*(M4-G4)/M4</f>
-        <v>7.1441662159154137E-2</v>
-      </c>
-      <c r="O4" s="23">
-        <v>157.14500000000001</v>
-      </c>
-      <c r="P4" s="24">
-        <f>100*(O4-$G$4)/O4</f>
-        <v>7.1441662159154137E-2</v>
-      </c>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="24" t="e">
-        <f>100*(Q4-$G$4)/Q4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S4" s="23"/>
-      <c r="T4" s="24" t="e">
-        <f>100*(S4-$G$4)/S4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U4" s="23"/>
-      <c r="V4" s="24" t="e">
-        <f>100*(U4-$G$4)/U4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W4" s="23"/>
-      <c r="X4" s="24" t="e">
-        <f>100*(W4-$G$4)/W4</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+        <f>100*(I4-G4)/G4</f>
+        <v>3.0736903751131559E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
@@ -928,55 +841,14 @@
         <v>34.708820000000003</v>
       </c>
       <c r="I5" s="22">
-        <v>45.341000000000001</v>
+        <v>37.462000000000003</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" si="0"/>
-        <v>30.632502055673449</v>
-      </c>
-      <c r="K5" s="22">
-        <v>39.938000000000002</v>
-      </c>
-      <c r="L5" s="24">
-        <f>100*(K5-$G$5)/K5</f>
-        <v>13.093244529019978</v>
-      </c>
-      <c r="M5" s="22">
-        <v>38.816000000000003</v>
-      </c>
-      <c r="N5" s="24">
-        <f t="shared" ref="N5:N10" si="1">100*(M5-G5)/M5</f>
-        <v>10.581152102225884</v>
-      </c>
-      <c r="O5" s="22">
-        <v>38.816000000000003</v>
-      </c>
-      <c r="P5" s="24">
-        <f t="shared" ref="P5" si="2">100*(O5-$G$4)/O5</f>
-        <v>-304.55671115004122</v>
-      </c>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="24" t="e">
-        <f t="shared" ref="R5" si="3">100*(Q5-$G$4)/Q5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S5" s="22"/>
-      <c r="T5" s="24" t="e">
-        <f t="shared" ref="T5" si="4">100*(S5-$G$4)/S5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U5" s="22"/>
-      <c r="V5" s="24" t="e">
-        <f t="shared" ref="V5" si="5">100*(U5-$G$4)/U5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W5" s="22"/>
-      <c r="X5" s="24" t="e">
-        <f t="shared" ref="X5" si="6">100*(W5-$G$4)/W5</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+        <f t="shared" ref="J5:J10" si="0">100*(I5-G5)/G5</f>
+        <v>7.9322201100469565</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>6</v>
       </c>
@@ -999,51 +871,14 @@
         <v>32.626666999999998</v>
       </c>
       <c r="I6" s="22">
-        <v>48.857999999999997</v>
+        <v>35.920999999999999</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="0"/>
-        <v>49.748670313152125</v>
-      </c>
-      <c r="K6" s="22">
-        <v>37.414999999999999</v>
-      </c>
-      <c r="L6" s="24">
-        <f>100*(K6-$G$6)/K6</f>
-        <v>12.79789656554858</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O6" s="22"/>
-      <c r="P6" s="24" t="e">
-        <f t="shared" ref="P6" si="7">100*(O6-$G$4)/O6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="24" t="e">
-        <f t="shared" ref="R6" si="8">100*(Q6-$G$4)/Q6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S6" s="22"/>
-      <c r="T6" s="24" t="e">
-        <f t="shared" ref="T6" si="9">100*(S6-$G$4)/S6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U6" s="22"/>
-      <c r="V6" s="24" t="e">
-        <f t="shared" ref="V6" si="10">100*(U6-$G$4)/U6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W6" s="22"/>
-      <c r="X6" s="24" t="e">
-        <f t="shared" ref="X6" si="11">100*(W6-$G$4)/W6</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+        <v>10.097056496760768</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
@@ -1065,52 +900,15 @@
       <c r="G7" s="10">
         <v>7.7172020000000003</v>
       </c>
-      <c r="I7" s="30">
-        <v>11.500999999999999</v>
+      <c r="I7" s="22">
+        <v>8.4120000000000008</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
-        <v>49.030697913570215</v>
-      </c>
-      <c r="K7" s="22">
-        <v>8.9920000000000009</v>
-      </c>
-      <c r="L7" s="24">
-        <f>100*(K7-$G$7)/K7</f>
-        <v>14.177024021352318</v>
-      </c>
-      <c r="M7" s="22"/>
-      <c r="N7" s="24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O7" s="22"/>
-      <c r="P7" s="24" t="e">
-        <f t="shared" ref="P7" si="12">100*(O7-$G$4)/O7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="24" t="e">
-        <f t="shared" ref="R7" si="13">100*(Q7-$G$4)/Q7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S7" s="22"/>
-      <c r="T7" s="24" t="e">
-        <f t="shared" ref="T7" si="14">100*(S7-$G$4)/S7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U7" s="22"/>
-      <c r="V7" s="24" t="e">
-        <f t="shared" ref="V7" si="15">100*(U7-$G$4)/U7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W7" s="22"/>
-      <c r="X7" s="24" t="e">
-        <f t="shared" ref="X7" si="16">100*(W7-$G$4)/W7</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+        <v>9.0032371836321037</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>8</v>
       </c>
@@ -1133,51 +931,14 @@
         <v>12.901103000000001</v>
       </c>
       <c r="I8" s="22">
-        <v>18.138000000000002</v>
+        <v>14.526999999999999</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>40.59262994799748</v>
-      </c>
-      <c r="K8" s="22">
-        <v>15.346</v>
-      </c>
-      <c r="L8" s="24">
-        <f>100*(K8-$G$8)/K8</f>
-        <v>15.931819366610187</v>
-      </c>
-      <c r="M8" s="22"/>
-      <c r="N8" s="24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="24" t="e">
-        <f t="shared" ref="P8" si="17">100*(O8-$G$4)/O8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="24" t="e">
-        <f t="shared" ref="R8" si="18">100*(Q8-$G$4)/Q8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S8" s="22"/>
-      <c r="T8" s="24" t="e">
-        <f t="shared" ref="T8" si="19">100*(S8-$G$4)/S8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U8" s="22"/>
-      <c r="V8" s="24" t="e">
-        <f t="shared" ref="V8" si="20">100*(U8-$G$4)/U8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W8" s="22"/>
-      <c r="X8" s="24" t="e">
-        <f t="shared" ref="X8" si="21">100*(W8-$G$4)/W8</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+        <v>12.602775127056951</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>9</v>
       </c>
@@ -1199,52 +960,15 @@
       <c r="G9" s="10">
         <v>3.044578</v>
       </c>
-      <c r="I9" s="29">
-        <v>4.6239999999999997</v>
+      <c r="I9" s="22">
+        <v>3.6309999999999998</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="0"/>
-        <v>51.87654906525632</v>
-      </c>
-      <c r="K9" s="22">
-        <v>3.645</v>
-      </c>
-      <c r="L9" s="24">
-        <f>100*(K9-$G$9)/K9</f>
-        <v>16.472482853223593</v>
-      </c>
-      <c r="M9" s="22"/>
-      <c r="N9" s="24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="24" t="e">
-        <f t="shared" ref="P9" si="22">100*(O9-$G$4)/O9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="24" t="e">
-        <f t="shared" ref="R9" si="23">100*(Q9-$G$4)/Q9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S9" s="22"/>
-      <c r="T9" s="24" t="e">
-        <f t="shared" ref="T9" si="24">100*(S9-$G$4)/S9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U9" s="22"/>
-      <c r="V9" s="24" t="e">
-        <f t="shared" ref="V9" si="25">100*(U9-$G$4)/U9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W9" s="22"/>
-      <c r="X9" s="24" t="e">
-        <f t="shared" ref="X9" si="26">100*(W9-$G$4)/W9</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>19.261191534590335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>10</v>
       </c>
@@ -1267,239 +991,65 @@
         <v>10.050300999999999</v>
       </c>
       <c r="I10" s="22">
-        <v>14.057</v>
+        <v>10.475</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>39.866457730967475</v>
-      </c>
-      <c r="K10" s="22">
-        <v>11.225</v>
-      </c>
-      <c r="L10" s="24">
-        <f>100*(K10-$G$10)/K10</f>
-        <v>10.465024498886418</v>
-      </c>
-      <c r="M10" s="22">
-        <v>11.007999999999999</v>
-      </c>
-      <c r="N10" s="24">
-        <f>100*(M10-G10)/M10</f>
-        <v>8.7000272529069758</v>
-      </c>
-      <c r="O10" s="22"/>
-      <c r="P10" s="24" t="e">
-        <f t="shared" ref="P10" si="27">100*(O10-$G$4)/O10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="24" t="e">
-        <f t="shared" ref="R10" si="28">100*(Q10-$G$4)/Q10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S10" s="22"/>
-      <c r="T10" s="24" t="e">
-        <f t="shared" ref="T10" si="29">100*(S10-$G$4)/S10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U10" s="22"/>
-      <c r="V10" s="24" t="e">
-        <f t="shared" ref="V10" si="30">100*(U10-$G$4)/U10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W10" s="22"/>
-      <c r="X10" s="24" t="e">
-        <f t="shared" ref="X10" si="31">100*(W10-$G$4)/W10</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+        <v>4.2257341347289046</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J12" s="4">
         <f>MIN(J4:J10)</f>
-        <v>6.3472543651137956</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="4">
-        <f t="shared" ref="L12" si="32">MIN(L4:L10)</f>
-        <v>0.39406992527940232</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12" s="4" t="e">
-        <f t="shared" ref="N12" si="33">MIN(N4:N10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P12" s="4" t="e">
-        <f t="shared" ref="P12" si="34">MIN(P4:P10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R12" s="4" t="e">
-        <f t="shared" ref="R12" si="35">MIN(R4:R10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T12" s="4" t="e">
-        <f t="shared" ref="T12" si="36">MIN(T4:T10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="V12" s="4" t="e">
-        <f t="shared" ref="V12" si="37">MIN(V4:V10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="X12" s="4" t="e">
-        <f t="shared" ref="X12" si="38">MIN(X4:X10)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+        <v>3.0736903751131559E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J13" s="4">
         <f>AVERAGE(J4:J10)</f>
-        <v>38.29925162739012</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="4">
-        <f t="shared" ref="L13" si="39">AVERAGE(L4:L10)</f>
-        <v>11.904508822845782</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N13" s="4" t="e">
-        <f t="shared" ref="N13" si="40">AVERAGE(N4:N10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P13" s="4" t="e">
-        <f t="shared" ref="P13" si="41">AVERAGE(P4:P10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R13" s="4" t="e">
-        <f t="shared" ref="R13" si="42">AVERAGE(R4:R10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="T13" s="4" t="e">
-        <f t="shared" ref="T13" si="43">AVERAGE(T4:T10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="V13" s="4" t="e">
-        <f t="shared" ref="V13" si="44">AVERAGE(V4:V10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="X13" s="4" t="e">
-        <f t="shared" ref="X13" si="45">AVERAGE(X4:X10)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+        <v>9.0218502129381655</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="J14" s="4">
         <f>MAX(J4:J10)</f>
-        <v>51.87654906525632</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" s="4">
-        <f t="shared" ref="L14" si="46">MAX(L4:L10)</f>
-        <v>16.472482853223593</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N14" s="4" t="e">
-        <f t="shared" ref="N14" si="47">MAX(N4:N10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P14" s="4" t="e">
-        <f t="shared" ref="P14" si="48">MAX(P4:P10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R14" s="4" t="e">
-        <f t="shared" ref="R14" si="49">MAX(R4:R10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T14" s="4" t="e">
-        <f t="shared" ref="T14" si="50">MAX(T4:T10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="V14" s="4" t="e">
-        <f t="shared" ref="V14" si="51">MAX(V4:V10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="X14" s="4" t="e">
-        <f t="shared" ref="X14" si="52">MAX(X4:X10)</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>19.261191534590335</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1507,12 +1057,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Final version sended to professors
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacopx/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacopx/Development/OMA_ExamTimeTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -731,7 +731,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -811,11 +811,11 @@
         <v>157.03273300000001</v>
       </c>
       <c r="I4" s="23">
-        <v>157.08099999999999</v>
+        <v>157.14500000000001</v>
       </c>
       <c r="J4" s="24">
         <f>100*(I4-G4)/G4</f>
-        <v>3.0736903751131559E-2</v>
+        <v>7.1492737759332486E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="J12" s="4">
         <f>MIN(J4:J10)</f>
-        <v>3.0736903751131559E-2</v>
+        <v>7.1492737759332486E-2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="J13" s="4">
         <f>AVERAGE(J4:J10)</f>
-        <v>9.0218502129381655</v>
+        <v>9.0276724749393349</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>